<commit_message>
+ add new word
</commit_message>
<xml_diff>
--- a/res/voc/animal.xlsx
+++ b/res/voc/animal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Động vật</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seen</t>
   </si>
   <si>
     <t xml:space="preserve">dog</t>
@@ -131,9 +134,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -207,7 +211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,6 +228,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -233,6 +241,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,14 +268,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,150 +293,185 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="C16" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="C17" s="8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C18" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>